<commit_message>
delete the reverse discitonary in get ovw descriptor cause it wasn't needed
</commit_message>
<xml_diff>
--- a/Configuration_file/RiskModel_ConfigurationFile.xlsx
+++ b/Configuration_file/RiskModel_ConfigurationFile.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DiegoBartoli\PycharmProjects\BusinessModel_app_generator\Configuration_settings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DiegoBartoli\PycharmProjects\BusinessModel_app_generator\Configuration_file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0635F573-94C5-41D1-9FB1-C940933DAB5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B263B5B-7C9E-4D59-B1C6-362F12C59FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="153">
   <si>
     <t>Page</t>
   </si>
@@ -487,6 +487,15 @@
   </si>
   <si>
     <t>Assesses  if you are leveraging all of the available information sources able to feed your risk program.  Scoring for this topic requires that you review all of the columns and count how many you cover. Use that count to assign your value as opposed to skipping by types.</t>
+  </si>
+  <si>
+    <t>RI Digitalization</t>
+  </si>
+  <si>
+    <t>RM Digitalization</t>
+  </si>
+  <si>
+    <t>SC Digitalization</t>
   </si>
 </sst>
 </file>
@@ -854,7 +863,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1428,7 +1437,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1547,7 +1556,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="D8" t="s">
         <v>147</v>
@@ -1603,7 +1612,7 @@
         <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>151</v>
       </c>
       <c r="D12" t="s">
         <v>148</v>
@@ -1659,7 +1668,7 @@
         <v>73</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>152</v>
       </c>
       <c r="D16" t="s">
         <v>148</v>

</xml_diff>

<commit_message>
Updated names and layout stuff
</commit_message>
<xml_diff>
--- a/Configuration_file/RiskModel_ConfigurationFile.xlsx
+++ b/Configuration_file/RiskModel_ConfigurationFile.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DiegoBartoli\PycharmProjects\BusinessModel_app_generator\Configuration_file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25E99B8-6348-40FD-A240-37D99F41B50D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD5BA40-7A18-4F8D-9C6A-36CFF9484FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelQuestions" sheetId="1" r:id="rId1"/>
     <sheet name="ModelOverview" sheetId="2" r:id="rId2"/>
+    <sheet name="ModelText" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,14 +38,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="154">
   <si>
     <t>Page</t>
   </si>
   <si>
-    <t>Tab</t>
-  </si>
-  <si>
     <t>Question</t>
   </si>
   <si>
@@ -405,9 +403,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Tab weight</t>
-  </si>
-  <si>
     <t>Page weight</t>
   </si>
   <si>
@@ -472,6 +467,39 @@
   </si>
   <si>
     <t>Performance management</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>This is the text for the:&lt;br&gt;**Home page**.</t>
+  </si>
+  <si>
+    <t>This is the text for the:&lt;br&gt;**Risk Identification page**.</t>
+  </si>
+  <si>
+    <t>This is the text for the:&lt;br&gt;**Risk Mitigation page**.</t>
+  </si>
+  <si>
+    <t>This is the text for the:&lt;br&gt;**Supplier Collaboration &amp; Network Resilience**.</t>
+  </si>
+  <si>
+    <t>This is the text for the:&lt;br&gt;**Organization, Governance &amp; Policies**.</t>
+  </si>
+  <si>
+    <t>Risk model assessment</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>Section weight</t>
   </si>
 </sst>
 </file>
@@ -838,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -858,548 +886,548 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="I6" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="G7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="G8" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="H8" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" t="s">
-        <v>130</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" t="s">
         <v>60</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>61</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>62</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>63</v>
-      </c>
-      <c r="I10" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" t="s">
         <v>65</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>66</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>67</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>68</v>
-      </c>
-      <c r="I11" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" t="s">
         <v>70</v>
       </c>
-      <c r="F12" t="s">
-        <v>71</v>
-      </c>
       <c r="G12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" t="s">
         <v>42</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>43</v>
-      </c>
-      <c r="I12" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" t="s">
+        <v>132</v>
+      </c>
+      <c r="E13" t="s">
         <v>72</v>
       </c>
-      <c r="B13" t="s">
-        <v>114</v>
-      </c>
-      <c r="D13" t="s">
-        <v>134</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>73</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>74</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>75</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>76</v>
-      </c>
-      <c r="I13" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" t="s">
+        <v>133</v>
+      </c>
+      <c r="E14" t="s">
         <v>72</v>
       </c>
-      <c r="B14" t="s">
-        <v>115</v>
-      </c>
-      <c r="D14" t="s">
-        <v>135</v>
-      </c>
-      <c r="E14" t="s">
-        <v>73</v>
-      </c>
       <c r="F14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G14" t="s">
         <v>78</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>79</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>80</v>
-      </c>
-      <c r="I14" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" t="s">
         <v>82</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>83</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>84</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>85</v>
-      </c>
-      <c r="I15" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" t="s">
         <v>42</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>43</v>
-      </c>
-      <c r="I16" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" t="s">
+        <v>135</v>
+      </c>
+      <c r="E17" t="s">
         <v>88</v>
       </c>
-      <c r="B17" t="s">
-        <v>117</v>
-      </c>
-      <c r="D17" t="s">
-        <v>137</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>89</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>90</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>91</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>92</v>
-      </c>
-      <c r="I17" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F18" t="s">
         <v>94</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>95</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>96</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>97</v>
-      </c>
-      <c r="I18" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D19" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E19" t="s">
+        <v>98</v>
+      </c>
+      <c r="F19" t="s">
         <v>99</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>100</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>101</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>102</v>
-      </c>
-      <c r="I19" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D20" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E20" t="s">
+        <v>103</v>
+      </c>
+      <c r="F20" t="s">
         <v>104</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>105</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>106</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>107</v>
-      </c>
-      <c r="I20" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B21" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D21" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E21" t="s">
+        <v>108</v>
+      </c>
+      <c r="F21" t="s">
         <v>109</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>110</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>111</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>112</v>
-      </c>
-      <c r="I21" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1413,7 +1441,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1430,180 +1458,262 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>152</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B21" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D6A044A-8FF1-4945-827B-BD32AAA0E079}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>